<commit_message>
atualização selec_respostas + survey
</commit_message>
<xml_diff>
--- a/my-app/public/respostas_questionarios.xlsx
+++ b/my-app/public/respostas_questionarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28221"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fteixeira\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pkfti.sharepoint.com/sites/IT-TEAM-Estagio_Curricular_FT/Documentos Partilhados/Estagio_Curricular_FT/App_Checklists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{09063D7B-8544-4842-876E-DF6744AF5D7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{62CEDB41-2849-4773-BA46-C68F41845599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D8C6A90-3449-4350-A9AB-75F2C7438A65}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B00370E6-9AA9-4AF8-B6CD-72F692D6C0E5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B00370E6-9AA9-4AF8-B6CD-72F692D6C0E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1233,7 +1233,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1328,10 +1328,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1680,22 +1676,22 @@
       <selection activeCell="G172" sqref="G13:G172"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" customWidth="1"/>
-    <col min="7" max="7" width="17.109375" customWidth="1"/>
-    <col min="8" max="8" width="35.5546875" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="35.5703125" customWidth="1"/>
     <col min="9" max="9" width="57" customWidth="1"/>
-    <col min="10" max="10" width="11.5546875" customWidth="1"/>
-    <col min="11" max="11" width="39.109375" customWidth="1"/>
-    <col min="12" max="12" width="26.88671875" customWidth="1"/>
-    <col min="13" max="13" width="15.33203125" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" customWidth="1"/>
+    <col min="11" max="11" width="39.140625" customWidth="1"/>
+    <col min="12" max="12" width="26.85546875" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1739,7 +1735,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="29.25">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -1763,7 +1759,7 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="29.25">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -1787,7 +1783,7 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
     </row>
-    <row r="4" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="29.25">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -1811,7 +1807,7 @@
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
     </row>
-    <row r="5" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="29.25">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -1835,7 +1831,7 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
     </row>
-    <row r="6" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="29.25">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -1859,7 +1855,7 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="29.25">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -1883,7 +1879,7 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="29.25">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -1907,7 +1903,7 @@
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
     </row>
-    <row r="9" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="29.25">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -1931,7 +1927,7 @@
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
     </row>
-    <row r="10" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="29.25">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -1955,7 +1951,7 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
     </row>
-    <row r="11" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="29.25">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -1979,7 +1975,7 @@
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
     </row>
-    <row r="12" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="29.25">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -2003,7 +1999,7 @@
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
     </row>
-    <row r="13" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="115.5">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -2029,7 +2025,7 @@
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
     </row>
-    <row r="14" spans="1:14" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="188.25">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -2055,7 +2051,7 @@
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
     </row>
-    <row r="15" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="130.5">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -2081,7 +2077,7 @@
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
     </row>
-    <row r="16" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="130.5">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -2107,7 +2103,7 @@
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
     </row>
-    <row r="17" spans="1:14" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" ht="159">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -2133,7 +2129,7 @@
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
     </row>
-    <row r="18" spans="1:14" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" ht="159">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
@@ -2159,7 +2155,7 @@
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
     </row>
-    <row r="19" spans="1:14" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" ht="174">
       <c r="A19" s="1" t="s">
         <v>14</v>
       </c>
@@ -2185,7 +2181,7 @@
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
     </row>
-    <row r="20" spans="1:14" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" ht="409.6">
       <c r="A20" s="1" t="s">
         <v>14</v>
       </c>
@@ -2211,7 +2207,7 @@
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
     </row>
-    <row r="21" spans="1:14" ht="331.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="346.5">
       <c r="A21" s="1" t="s">
         <v>14</v>
       </c>
@@ -2237,7 +2233,7 @@
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
     </row>
-    <row r="22" spans="1:14" ht="302.39999999999998" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" ht="303.75">
       <c r="A22" s="1" t="s">
         <v>14</v>
       </c>
@@ -2263,7 +2259,7 @@
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
     </row>
-    <row r="23" spans="1:14" ht="144" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" ht="159">
       <c r="A23" s="1" t="s">
         <v>14</v>
       </c>
@@ -2289,7 +2285,7 @@
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
     </row>
-    <row r="24" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" ht="115.5">
       <c r="A24" s="1" t="s">
         <v>14</v>
       </c>
@@ -2315,7 +2311,7 @@
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
     </row>
-    <row r="25" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" ht="130.5">
       <c r="A25" s="1" t="s">
         <v>14</v>
       </c>
@@ -2341,7 +2337,7 @@
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
     </row>
-    <row r="26" spans="1:14" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" ht="159">
       <c r="A26" s="1" t="s">
         <v>14</v>
       </c>
@@ -2367,7 +2363,7 @@
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
     </row>
-    <row r="27" spans="1:14" ht="144" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" ht="159">
       <c r="A27" s="1" t="s">
         <v>14</v>
       </c>
@@ -2393,7 +2389,7 @@
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
     </row>
-    <row r="28" spans="1:14" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" ht="216.75">
       <c r="A28" s="1" t="s">
         <v>14</v>
       </c>
@@ -2419,7 +2415,7 @@
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
     </row>
-    <row r="29" spans="1:14" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" ht="188.25">
       <c r="A29" s="1" t="s">
         <v>14</v>
       </c>
@@ -2445,7 +2441,7 @@
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
     </row>
-    <row r="30" spans="1:14" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" ht="174">
       <c r="A30" s="1" t="s">
         <v>14</v>
       </c>
@@ -2471,7 +2467,7 @@
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
     </row>
-    <row r="31" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" ht="159">
       <c r="A31" s="1" t="s">
         <v>14</v>
       </c>
@@ -2497,7 +2493,7 @@
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
     </row>
-    <row r="32" spans="1:14" ht="144" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" ht="144.75">
       <c r="A32" s="1" t="s">
         <v>14</v>
       </c>
@@ -2523,7 +2519,7 @@
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
     </row>
-    <row r="33" spans="1:14" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" ht="159">
       <c r="A33" s="1" t="s">
         <v>14</v>
       </c>
@@ -2549,7 +2545,7 @@
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
     </row>
-    <row r="34" spans="1:14" ht="144" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" ht="144.75">
       <c r="A34" s="1" t="s">
         <v>14</v>
       </c>
@@ -2575,7 +2571,7 @@
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
     </row>
-    <row r="35" spans="1:14" ht="144" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" ht="144.75">
       <c r="A35" s="1" t="s">
         <v>14</v>
       </c>
@@ -2601,7 +2597,7 @@
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
     </row>
-    <row r="36" spans="1:14" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" ht="174">
       <c r="A36" s="1" t="s">
         <v>14</v>
       </c>
@@ -2627,7 +2623,7 @@
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
     </row>
-    <row r="37" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" ht="115.5">
       <c r="A37" s="1" t="s">
         <v>14</v>
       </c>
@@ -2653,7 +2649,7 @@
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
     </row>
-    <row r="38" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" ht="144.75">
       <c r="A38" s="1" t="s">
         <v>14</v>
       </c>
@@ -2679,7 +2675,7 @@
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
     </row>
-    <row r="39" spans="1:14" ht="144" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" ht="144.75">
       <c r="A39" s="1" t="s">
         <v>14</v>
       </c>
@@ -2705,7 +2701,7 @@
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
     </row>
-    <row r="40" spans="1:14" ht="144" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" ht="159">
       <c r="A40" s="1" t="s">
         <v>14</v>
       </c>
@@ -2731,7 +2727,7 @@
       <c r="M40" s="1"/>
       <c r="N40" s="1"/>
     </row>
-    <row r="41" spans="1:14" ht="144" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" ht="144.75">
       <c r="A41" s="1" t="s">
         <v>14</v>
       </c>
@@ -2757,7 +2753,7 @@
       <c r="M41" s="1"/>
       <c r="N41" s="1"/>
     </row>
-    <row r="42" spans="1:14" ht="144" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" ht="159">
       <c r="A42" s="1" t="s">
         <v>14</v>
       </c>
@@ -2783,7 +2779,7 @@
       <c r="M42" s="1"/>
       <c r="N42" s="1"/>
     </row>
-    <row r="43" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" ht="101.25">
       <c r="A43" s="1" t="s">
         <v>14</v>
       </c>
@@ -2809,7 +2805,7 @@
       <c r="M43" s="1"/>
       <c r="N43" s="1"/>
     </row>
-    <row r="44" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" ht="144.75">
       <c r="A44" s="1" t="s">
         <v>14</v>
       </c>
@@ -2835,7 +2831,7 @@
       <c r="M44" s="1"/>
       <c r="N44" s="1"/>
     </row>
-    <row r="45" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" ht="87">
       <c r="A45" s="1" t="s">
         <v>14</v>
       </c>
@@ -2861,7 +2857,7 @@
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
     </row>
-    <row r="46" spans="1:14" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14" ht="201.75">
       <c r="A46" s="1" t="s">
         <v>14</v>
       </c>
@@ -2887,7 +2883,7 @@
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
     </row>
-    <row r="47" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" ht="144.75">
       <c r="A47" s="1" t="s">
         <v>14</v>
       </c>
@@ -2913,7 +2909,7 @@
       <c r="M47" s="1"/>
       <c r="N47" s="1"/>
     </row>
-    <row r="48" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:14" ht="144.75">
       <c r="A48" s="1" t="s">
         <v>14</v>
       </c>
@@ -2939,7 +2935,7 @@
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
     </row>
-    <row r="49" spans="1:14" ht="144" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:14" ht="144.75">
       <c r="A49" s="1" t="s">
         <v>14</v>
       </c>
@@ -2965,7 +2961,7 @@
       <c r="M49" s="1"/>
       <c r="N49" s="1"/>
     </row>
-    <row r="50" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:14" ht="130.5">
       <c r="A50" s="1" t="s">
         <v>14</v>
       </c>
@@ -2991,7 +2987,7 @@
       <c r="M50" s="1"/>
       <c r="N50" s="1"/>
     </row>
-    <row r="51" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" ht="130.5">
       <c r="A51" s="1" t="s">
         <v>14</v>
       </c>
@@ -3017,7 +3013,7 @@
       <c r="M51" s="1"/>
       <c r="N51" s="1"/>
     </row>
-    <row r="52" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:14" ht="101.25">
       <c r="A52" s="1" t="s">
         <v>14</v>
       </c>
@@ -3043,7 +3039,7 @@
       <c r="M52" s="1"/>
       <c r="N52" s="1"/>
     </row>
-    <row r="53" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:14" ht="130.5">
       <c r="A53" s="1" t="s">
         <v>14</v>
       </c>
@@ -3069,7 +3065,7 @@
       <c r="M53" s="1"/>
       <c r="N53" s="1"/>
     </row>
-    <row r="54" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:14" ht="130.5">
       <c r="A54" s="1" t="s">
         <v>14</v>
       </c>
@@ -3095,7 +3091,7 @@
       <c r="M54" s="1"/>
       <c r="N54" s="1"/>
     </row>
-    <row r="55" spans="1:14" ht="144" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:14" ht="144.75">
       <c r="A55" s="1" t="s">
         <v>14</v>
       </c>
@@ -3121,7 +3117,7 @@
       <c r="M55" s="1"/>
       <c r="N55" s="1"/>
     </row>
-    <row r="56" spans="1:14" ht="216" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:14" ht="216.75">
       <c r="A56" s="1" t="s">
         <v>14</v>
       </c>
@@ -3147,7 +3143,7 @@
       <c r="M56" s="1"/>
       <c r="N56" s="1"/>
     </row>
-    <row r="57" spans="1:14" ht="302.39999999999998" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:14" ht="303.75">
       <c r="A57" s="1" t="s">
         <v>14</v>
       </c>
@@ -3173,7 +3169,7 @@
       <c r="M57" s="1"/>
       <c r="N57" s="1"/>
     </row>
-    <row r="58" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:14" ht="87">
       <c r="A58" s="1" t="s">
         <v>14</v>
       </c>
@@ -3199,7 +3195,7 @@
       <c r="M58" s="1"/>
       <c r="N58" s="1"/>
     </row>
-    <row r="59" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:14" ht="115.5">
       <c r="A59" s="1" t="s">
         <v>14</v>
       </c>
@@ -3225,7 +3221,7 @@
       <c r="M59" s="1"/>
       <c r="N59" s="1"/>
     </row>
-    <row r="60" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:14" ht="130.5">
       <c r="A60" s="1" t="s">
         <v>14</v>
       </c>
@@ -3251,7 +3247,7 @@
       <c r="M60" s="1"/>
       <c r="N60" s="1"/>
     </row>
-    <row r="61" spans="1:14" ht="144" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:14" ht="144.75">
       <c r="A61" s="1" t="s">
         <v>14</v>
       </c>
@@ -3277,7 +3273,7 @@
       <c r="M61" s="1"/>
       <c r="N61" s="1"/>
     </row>
-    <row r="62" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:14" ht="130.5">
       <c r="A62" s="1" t="s">
         <v>14</v>
       </c>
@@ -3303,7 +3299,7 @@
       <c r="M62" s="1"/>
       <c r="N62" s="1"/>
     </row>
-    <row r="63" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:14" ht="130.5">
       <c r="A63" s="1" t="s">
         <v>14</v>
       </c>
@@ -3329,7 +3325,7 @@
       <c r="M63" s="1"/>
       <c r="N63" s="1"/>
     </row>
-    <row r="64" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:14" ht="130.5">
       <c r="A64" s="1" t="s">
         <v>14</v>
       </c>
@@ -3355,7 +3351,7 @@
       <c r="M64" s="1"/>
       <c r="N64" s="1"/>
     </row>
-    <row r="65" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" ht="130.5">
       <c r="A65" s="1" t="s">
         <v>14</v>
       </c>
@@ -3381,7 +3377,7 @@
       <c r="M65" s="1"/>
       <c r="N65" s="1"/>
     </row>
-    <row r="66" spans="1:14" ht="288" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" ht="303.75">
       <c r="A66" s="1" t="s">
         <v>14</v>
       </c>
@@ -3407,7 +3403,7 @@
       <c r="M66" s="1"/>
       <c r="N66" s="1"/>
     </row>
-    <row r="67" spans="1:14" ht="316.8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" ht="318">
       <c r="A67" s="1" t="s">
         <v>14</v>
       </c>
@@ -3433,7 +3429,7 @@
       <c r="M67" s="1"/>
       <c r="N67" s="1"/>
     </row>
-    <row r="68" spans="1:14" ht="216" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:14" ht="245.25">
       <c r="A68" s="1" t="s">
         <v>14</v>
       </c>
@@ -3459,7 +3455,7 @@
       <c r="M68" s="1"/>
       <c r="N68" s="1"/>
     </row>
-    <row r="69" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:14" ht="101.25">
       <c r="A69" s="1" t="s">
         <v>14</v>
       </c>
@@ -3485,7 +3481,7 @@
       <c r="M69" s="1"/>
       <c r="N69" s="1"/>
     </row>
-    <row r="70" spans="1:14" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:14" ht="274.5">
       <c r="A70" s="1" t="s">
         <v>14</v>
       </c>
@@ -3511,7 +3507,7 @@
       <c r="M70" s="1"/>
       <c r="N70" s="1"/>
     </row>
-    <row r="71" spans="1:14" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:14" ht="245.25">
       <c r="A71" s="1" t="s">
         <v>14</v>
       </c>
@@ -3537,7 +3533,7 @@
       <c r="M71" s="1"/>
       <c r="N71" s="1"/>
     </row>
-    <row r="72" spans="1:14" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:14" ht="188.25">
       <c r="A72" s="1" t="s">
         <v>14</v>
       </c>
@@ -3563,7 +3559,7 @@
       <c r="M72" s="1"/>
       <c r="N72" s="1"/>
     </row>
-    <row r="73" spans="1:14" ht="216" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:14" ht="231">
       <c r="A73" s="1" t="s">
         <v>14</v>
       </c>
@@ -3589,7 +3585,7 @@
       <c r="M73" s="1"/>
       <c r="N73" s="1"/>
     </row>
-    <row r="74" spans="1:14" ht="144" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:14" ht="144.75">
       <c r="A74" s="1" t="s">
         <v>14</v>
       </c>
@@ -3615,7 +3611,7 @@
       <c r="M74" s="1"/>
       <c r="N74" s="1"/>
     </row>
-    <row r="75" spans="1:14" ht="144" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:14" ht="144.75">
       <c r="A75" s="1" t="s">
         <v>14</v>
       </c>
@@ -3641,7 +3637,7 @@
       <c r="M75" s="1"/>
       <c r="N75" s="1"/>
     </row>
-    <row r="76" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:14" ht="144.75">
       <c r="A76" s="1" t="s">
         <v>14</v>
       </c>
@@ -3667,7 +3663,7 @@
       <c r="M76" s="1"/>
       <c r="N76" s="1"/>
     </row>
-    <row r="77" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:14" ht="130.5">
       <c r="A77" s="1" t="s">
         <v>14</v>
       </c>
@@ -3693,7 +3689,7 @@
       <c r="M77" s="1"/>
       <c r="N77" s="1"/>
     </row>
-    <row r="78" spans="1:14" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:14" ht="174">
       <c r="A78" s="1" t="s">
         <v>14</v>
       </c>
@@ -3719,7 +3715,7 @@
       <c r="M78" s="1"/>
       <c r="N78" s="1"/>
     </row>
-    <row r="79" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:14" ht="130.5">
       <c r="A79" s="1" t="s">
         <v>14</v>
       </c>
@@ -3745,7 +3741,7 @@
       <c r="M79" s="1"/>
       <c r="N79" s="1"/>
     </row>
-    <row r="80" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:14" ht="115.5">
       <c r="A80" s="1" t="s">
         <v>14</v>
       </c>
@@ -3771,7 +3767,7 @@
       <c r="M80" s="1"/>
       <c r="N80" s="1"/>
     </row>
-    <row r="81" spans="1:14" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:14" ht="201.75">
       <c r="A81" s="1" t="s">
         <v>14</v>
       </c>
@@ -3797,7 +3793,7 @@
       <c r="M81" s="1"/>
       <c r="N81" s="1"/>
     </row>
-    <row r="82" spans="1:14" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:14" ht="188.25">
       <c r="A82" s="1" t="s">
         <v>14</v>
       </c>
@@ -3823,7 +3819,7 @@
       <c r="M82" s="1"/>
       <c r="N82" s="1"/>
     </row>
-    <row r="83" spans="1:14" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:14" ht="174">
       <c r="A83" s="1" t="s">
         <v>14</v>
       </c>
@@ -3849,7 +3845,7 @@
       <c r="M83" s="1"/>
       <c r="N83" s="1"/>
     </row>
-    <row r="84" spans="1:14" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:14" ht="159">
       <c r="A84" s="1" t="s">
         <v>14</v>
       </c>
@@ -3875,7 +3871,7 @@
       <c r="M84" s="1"/>
       <c r="N84" s="1"/>
     </row>
-    <row r="85" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:14" ht="115.5">
       <c r="A85" s="1" t="s">
         <v>14</v>
       </c>
@@ -3901,7 +3897,7 @@
       <c r="M85" s="1"/>
       <c r="N85" s="1"/>
     </row>
-    <row r="86" spans="1:14" ht="144" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:14" ht="144.75">
       <c r="A86" s="1" t="s">
         <v>14</v>
       </c>
@@ -3927,7 +3923,7 @@
       <c r="M86" s="1"/>
       <c r="N86" s="1"/>
     </row>
-    <row r="87" spans="1:14" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:14" ht="174">
       <c r="A87" s="1" t="s">
         <v>14</v>
       </c>
@@ -3953,7 +3949,7 @@
       <c r="M87" s="1"/>
       <c r="N87" s="1"/>
     </row>
-    <row r="88" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:14" ht="72.75">
       <c r="A88" s="1" t="s">
         <v>14</v>
       </c>
@@ -3979,7 +3975,7 @@
       <c r="M88" s="1"/>
       <c r="N88" s="1"/>
     </row>
-    <row r="89" spans="1:14" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:14" ht="188.25">
       <c r="A89" s="1" t="s">
         <v>14</v>
       </c>
@@ -4005,7 +4001,7 @@
       <c r="M89" s="1"/>
       <c r="N89" s="1"/>
     </row>
-    <row r="90" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:14" ht="72.75">
       <c r="A90" s="1" t="s">
         <v>14</v>
       </c>
@@ -4031,7 +4027,7 @@
       <c r="M90" s="1"/>
       <c r="N90" s="1"/>
     </row>
-    <row r="91" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:14" ht="115.5">
       <c r="A91" s="1" t="s">
         <v>14</v>
       </c>
@@ -4057,7 +4053,7 @@
       <c r="M91" s="1"/>
       <c r="N91" s="1"/>
     </row>
-    <row r="92" spans="1:14" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:14" ht="159">
       <c r="A92" s="1" t="s">
         <v>14</v>
       </c>
@@ -4083,7 +4079,7 @@
       <c r="M92" s="1"/>
       <c r="N92" s="1"/>
     </row>
-    <row r="93" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:14" ht="144.75">
       <c r="A93" s="1" t="s">
         <v>14</v>
       </c>
@@ -4109,7 +4105,7 @@
       <c r="M93" s="1"/>
       <c r="N93" s="1"/>
     </row>
-    <row r="94" spans="1:14" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:14" ht="174">
       <c r="A94" s="1" t="s">
         <v>14</v>
       </c>
@@ -4135,7 +4131,7 @@
       <c r="M94" s="1"/>
       <c r="N94" s="1"/>
     </row>
-    <row r="95" spans="1:14" ht="144" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:14" ht="144.75">
       <c r="A95" s="1" t="s">
         <v>14</v>
       </c>
@@ -4161,7 +4157,7 @@
       <c r="M95" s="1"/>
       <c r="N95" s="1"/>
     </row>
-    <row r="96" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:14" ht="130.5">
       <c r="A96" s="1" t="s">
         <v>14</v>
       </c>
@@ -4187,7 +4183,7 @@
       <c r="M96" s="1"/>
       <c r="N96" s="1"/>
     </row>
-    <row r="97" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:14" ht="87">
       <c r="A97" s="1" t="s">
         <v>14</v>
       </c>
@@ -4213,7 +4209,7 @@
       <c r="M97" s="1"/>
       <c r="N97" s="1"/>
     </row>
-    <row r="98" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:14" ht="101.25">
       <c r="A98" s="1" t="s">
         <v>14</v>
       </c>
@@ -4239,7 +4235,7 @@
       <c r="M98" s="1"/>
       <c r="N98" s="1"/>
     </row>
-    <row r="99" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:14" ht="130.5">
       <c r="A99" s="1" t="s">
         <v>14</v>
       </c>
@@ -4265,7 +4261,7 @@
       <c r="M99" s="1"/>
       <c r="N99" s="1"/>
     </row>
-    <row r="100" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:14" ht="130.5">
       <c r="A100" s="1" t="s">
         <v>14</v>
       </c>
@@ -4291,7 +4287,7 @@
       <c r="M100" s="1"/>
       <c r="N100" s="1"/>
     </row>
-    <row r="101" spans="1:14" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:14" ht="174">
       <c r="A101" s="1" t="s">
         <v>14</v>
       </c>
@@ -4317,7 +4313,7 @@
       <c r="M101" s="1"/>
       <c r="N101" s="1"/>
     </row>
-    <row r="102" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:14" ht="144.75">
       <c r="A102" s="1" t="s">
         <v>14</v>
       </c>
@@ -4343,7 +4339,7 @@
       <c r="M102" s="1"/>
       <c r="N102" s="1"/>
     </row>
-    <row r="103" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:14" ht="101.25">
       <c r="A103" s="1" t="s">
         <v>14</v>
       </c>
@@ -4369,7 +4365,7 @@
       <c r="M103" s="1"/>
       <c r="N103" s="1"/>
     </row>
-    <row r="104" spans="1:14" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:14" ht="159">
       <c r="A104" s="1" t="s">
         <v>14</v>
       </c>
@@ -4395,7 +4391,7 @@
       <c r="M104" s="1"/>
       <c r="N104" s="1"/>
     </row>
-    <row r="105" spans="1:14" ht="144" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:14" ht="159">
       <c r="A105" s="1" t="s">
         <v>14</v>
       </c>
@@ -4421,7 +4417,7 @@
       <c r="M105" s="1"/>
       <c r="N105" s="1"/>
     </row>
-    <row r="106" spans="1:14" ht="216" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:14" ht="245.25">
       <c r="A106" s="1" t="s">
         <v>14</v>
       </c>
@@ -4447,7 +4443,7 @@
       <c r="M106" s="1"/>
       <c r="N106" s="1"/>
     </row>
-    <row r="107" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:14" ht="130.5">
       <c r="A107" s="1" t="s">
         <v>14</v>
       </c>
@@ -4473,7 +4469,7 @@
       <c r="M107" s="1"/>
       <c r="N107" s="1"/>
     </row>
-    <row r="108" spans="1:14" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:14" ht="288.75">
       <c r="A108" s="1" t="s">
         <v>14</v>
       </c>
@@ -4499,7 +4495,7 @@
       <c r="M108" s="1"/>
       <c r="N108" s="1"/>
     </row>
-    <row r="109" spans="1:14" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:14" ht="274.5">
       <c r="A109" s="1" t="s">
         <v>14</v>
       </c>
@@ -4525,7 +4521,7 @@
       <c r="M109" s="1"/>
       <c r="N109" s="1"/>
     </row>
-    <row r="110" spans="1:14" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:14" ht="274.5">
       <c r="A110" s="1" t="s">
         <v>14</v>
       </c>
@@ -4551,7 +4547,7 @@
       <c r="M110" s="1"/>
       <c r="N110" s="1"/>
     </row>
-    <row r="111" spans="1:14" ht="216" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:14" ht="231">
       <c r="A111" s="1" t="s">
         <v>14</v>
       </c>
@@ -4577,7 +4573,7 @@
       <c r="M111" s="1"/>
       <c r="N111" s="1"/>
     </row>
-    <row r="112" spans="1:14" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:14" ht="274.5">
       <c r="A112" s="1" t="s">
         <v>14</v>
       </c>
@@ -4603,7 +4599,7 @@
       <c r="M112" s="1"/>
       <c r="N112" s="1"/>
     </row>
-    <row r="113" spans="1:14" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:14" ht="174">
       <c r="A113" s="1" t="s">
         <v>14</v>
       </c>
@@ -4629,7 +4625,7 @@
       <c r="M113" s="1"/>
       <c r="N113" s="1"/>
     </row>
-    <row r="114" spans="1:14" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:14" ht="274.5">
       <c r="A114" s="1" t="s">
         <v>14</v>
       </c>
@@ -4655,7 +4651,7 @@
       <c r="M114" s="1"/>
       <c r="N114" s="1"/>
     </row>
-    <row r="115" spans="1:14" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:14" ht="260.25">
       <c r="A115" s="1" t="s">
         <v>14</v>
       </c>
@@ -4681,7 +4677,7 @@
       <c r="M115" s="1"/>
       <c r="N115" s="1"/>
     </row>
-    <row r="116" spans="1:14" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:14" ht="245.25">
       <c r="A116" s="1" t="s">
         <v>14</v>
       </c>
@@ -4707,7 +4703,7 @@
       <c r="M116" s="1"/>
       <c r="N116" s="1"/>
     </row>
-    <row r="117" spans="1:14" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:14" ht="188.25">
       <c r="A117" s="1" t="s">
         <v>14</v>
       </c>
@@ -4733,7 +4729,7 @@
       <c r="M117" s="1"/>
       <c r="N117" s="1"/>
     </row>
-    <row r="118" spans="1:14" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:14" ht="201.75">
       <c r="A118" s="1" t="s">
         <v>14</v>
       </c>
@@ -4759,7 +4755,7 @@
       <c r="M118" s="1"/>
       <c r="N118" s="1"/>
     </row>
-    <row r="119" spans="1:14" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:14" ht="274.5">
       <c r="A119" s="1" t="s">
         <v>14</v>
       </c>
@@ -4785,7 +4781,7 @@
       <c r="M119" s="1"/>
       <c r="N119" s="1"/>
     </row>
-    <row r="120" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:14" ht="87">
       <c r="A120" s="1" t="s">
         <v>14</v>
       </c>
@@ -4811,7 +4807,7 @@
       <c r="M120" s="1"/>
       <c r="N120" s="1"/>
     </row>
-    <row r="121" spans="1:14" ht="216" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:14" ht="216.75">
       <c r="A121" s="1" t="s">
         <v>14</v>
       </c>
@@ -4837,7 +4833,7 @@
       <c r="M121" s="1"/>
       <c r="N121" s="1"/>
     </row>
-    <row r="122" spans="1:14" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:14" ht="201.75">
       <c r="A122" s="1" t="s">
         <v>14</v>
       </c>
@@ -4863,7 +4859,7 @@
       <c r="M122" s="1"/>
       <c r="N122" s="1"/>
     </row>
-    <row r="123" spans="1:14" ht="288" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:14" ht="288.75">
       <c r="A123" s="1" t="s">
         <v>14</v>
       </c>
@@ -4889,7 +4885,7 @@
       <c r="M123" s="1"/>
       <c r="N123" s="1"/>
     </row>
-    <row r="124" spans="1:14" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:14" ht="216.75">
       <c r="A124" s="1" t="s">
         <v>14</v>
       </c>
@@ -4915,7 +4911,7 @@
       <c r="M124" s="1"/>
       <c r="N124" s="1"/>
     </row>
-    <row r="125" spans="1:14" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:14" ht="409.6">
       <c r="A125" s="1" t="s">
         <v>14</v>
       </c>
@@ -4941,7 +4937,7 @@
       <c r="M125" s="1"/>
       <c r="N125" s="1"/>
     </row>
-    <row r="126" spans="1:14" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:14" ht="274.5">
       <c r="A126" s="1" t="s">
         <v>14</v>
       </c>
@@ -4967,7 +4963,7 @@
       <c r="M126" s="1"/>
       <c r="N126" s="1"/>
     </row>
-    <row r="127" spans="1:14" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:14" ht="159">
       <c r="A127" s="1" t="s">
         <v>14</v>
       </c>
@@ -4993,7 +4989,7 @@
       <c r="M127" s="1"/>
       <c r="N127" s="1"/>
     </row>
-    <row r="128" spans="1:14" ht="216" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:14" ht="216.75">
       <c r="A128" s="1" t="s">
         <v>14</v>
       </c>
@@ -5019,7 +5015,7 @@
       <c r="M128" s="1"/>
       <c r="N128" s="1"/>
     </row>
-    <row r="129" spans="1:14" ht="144" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:14" ht="174">
       <c r="A129" s="1" t="s">
         <v>14</v>
       </c>
@@ -5045,7 +5041,7 @@
       <c r="M129" s="1"/>
       <c r="N129" s="1"/>
     </row>
-    <row r="130" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:14" ht="130.5">
       <c r="A130" s="1" t="s">
         <v>14</v>
       </c>
@@ -5071,7 +5067,7 @@
       <c r="M130" s="1"/>
       <c r="N130" s="1"/>
     </row>
-    <row r="131" spans="1:14" ht="144" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:14" ht="159">
       <c r="A131" s="1" t="s">
         <v>14</v>
       </c>
@@ -5097,7 +5093,7 @@
       <c r="M131" s="1"/>
       <c r="N131" s="1"/>
     </row>
-    <row r="132" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:14" ht="130.5">
       <c r="A132" s="1" t="s">
         <v>14</v>
       </c>
@@ -5123,7 +5119,7 @@
       <c r="M132" s="1"/>
       <c r="N132" s="1"/>
     </row>
-    <row r="133" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:14" ht="144.75">
       <c r="A133" s="1" t="s">
         <v>14</v>
       </c>
@@ -5149,7 +5145,7 @@
       <c r="M133" s="1"/>
       <c r="N133" s="1"/>
     </row>
-    <row r="134" spans="1:14" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:14" ht="174">
       <c r="A134" s="1" t="s">
         <v>14</v>
       </c>
@@ -5175,7 +5171,7 @@
       <c r="M134" s="1"/>
       <c r="N134" s="1"/>
     </row>
-    <row r="135" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:14" ht="115.5">
       <c r="A135" s="1" t="s">
         <v>14</v>
       </c>
@@ -5201,7 +5197,7 @@
       <c r="M135" s="1"/>
       <c r="N135" s="1"/>
     </row>
-    <row r="136" spans="1:14" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:14" ht="201.75">
       <c r="A136" s="1" t="s">
         <v>14</v>
       </c>
@@ -5227,7 +5223,7 @@
       <c r="M136" s="1"/>
       <c r="N136" s="1"/>
     </row>
-    <row r="137" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:14" ht="130.5">
       <c r="A137" s="1" t="s">
         <v>14</v>
       </c>
@@ -5253,7 +5249,7 @@
       <c r="M137" s="1"/>
       <c r="N137" s="1"/>
     </row>
-    <row r="138" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:14" ht="57.75">
       <c r="A138" s="1" t="s">
         <v>14</v>
       </c>
@@ -5279,7 +5275,7 @@
       <c r="M138" s="1"/>
       <c r="N138" s="1"/>
     </row>
-    <row r="139" spans="1:14" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:14" ht="188.25">
       <c r="A139" s="1" t="s">
         <v>14</v>
       </c>
@@ -5305,7 +5301,7 @@
       <c r="M139" s="1"/>
       <c r="N139" s="1"/>
     </row>
-    <row r="140" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:14" ht="130.5">
       <c r="A140" s="1" t="s">
         <v>14</v>
       </c>
@@ -5331,7 +5327,7 @@
       <c r="M140" s="1"/>
       <c r="N140" s="1"/>
     </row>
-    <row r="141" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:14" ht="144.75">
       <c r="A141" s="1" t="s">
         <v>14</v>
       </c>
@@ -5357,7 +5353,7 @@
       <c r="M141" s="1"/>
       <c r="N141" s="1"/>
     </row>
-    <row r="142" spans="1:14" ht="144" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:14" ht="159">
       <c r="A142" s="1" t="s">
         <v>14</v>
       </c>
@@ -5383,7 +5379,7 @@
       <c r="M142" s="1"/>
       <c r="N142" s="1"/>
     </row>
-    <row r="143" spans="1:14" ht="144" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:14" ht="144.75">
       <c r="A143" s="1" t="s">
         <v>14</v>
       </c>
@@ -5409,7 +5405,7 @@
       <c r="M143" s="1"/>
       <c r="N143" s="1"/>
     </row>
-    <row r="144" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:14" ht="130.5">
       <c r="A144" s="1" t="s">
         <v>14</v>
       </c>
@@ -5435,7 +5431,7 @@
       <c r="M144" s="1"/>
       <c r="N144" s="1"/>
     </row>
-    <row r="145" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:14" ht="144.75">
       <c r="A145" s="1" t="s">
         <v>14</v>
       </c>
@@ -5461,7 +5457,7 @@
       <c r="M145" s="1"/>
       <c r="N145" s="1"/>
     </row>
-    <row r="146" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:14" ht="144.75">
       <c r="A146" s="1" t="s">
         <v>14</v>
       </c>
@@ -5487,7 +5483,7 @@
       <c r="M146" s="1"/>
       <c r="N146" s="1"/>
     </row>
-    <row r="147" spans="1:14" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:14" ht="159">
       <c r="A147" s="1" t="s">
         <v>14</v>
       </c>
@@ -5513,7 +5509,7 @@
       <c r="M147" s="1"/>
       <c r="N147" s="1"/>
     </row>
-    <row r="148" spans="1:14" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:14" ht="159">
       <c r="A148" s="1" t="s">
         <v>14</v>
       </c>
@@ -5539,7 +5535,7 @@
       <c r="M148" s="1"/>
       <c r="N148" s="1"/>
     </row>
-    <row r="149" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:14" ht="144.75">
       <c r="A149" s="1" t="s">
         <v>14</v>
       </c>
@@ -5565,7 +5561,7 @@
       <c r="M149" s="1"/>
       <c r="N149" s="1"/>
     </row>
-    <row r="150" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:14" ht="87">
       <c r="A150" s="1" t="s">
         <v>14</v>
       </c>
@@ -5591,7 +5587,7 @@
       <c r="M150" s="1"/>
       <c r="N150" s="1"/>
     </row>
-    <row r="151" spans="1:14" ht="144" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:14" ht="144.75">
       <c r="A151" s="1" t="s">
         <v>14</v>
       </c>
@@ -5617,7 +5613,7 @@
       <c r="M151" s="1"/>
       <c r="N151" s="1"/>
     </row>
-    <row r="152" spans="1:14" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:14" ht="188.25">
       <c r="A152" s="1" t="s">
         <v>14</v>
       </c>
@@ -5643,7 +5639,7 @@
       <c r="M152" s="1"/>
       <c r="N152" s="1"/>
     </row>
-    <row r="153" spans="1:14" ht="144" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:14" ht="144.75">
       <c r="A153" s="1" t="s">
         <v>14</v>
       </c>
@@ -5669,7 +5665,7 @@
       <c r="M153" s="1"/>
       <c r="N153" s="1"/>
     </row>
-    <row r="154" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:14" ht="87">
       <c r="A154" s="1" t="s">
         <v>14</v>
       </c>
@@ -5695,7 +5691,7 @@
       <c r="M154" s="1"/>
       <c r="N154" s="1"/>
     </row>
-    <row r="155" spans="1:14" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:14" ht="260.25">
       <c r="A155" s="1" t="s">
         <v>14</v>
       </c>
@@ -5721,7 +5717,7 @@
       <c r="M155" s="1"/>
       <c r="N155" s="1"/>
     </row>
-    <row r="156" spans="1:14" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:14" ht="159">
       <c r="A156" s="1" t="s">
         <v>14</v>
       </c>
@@ -5747,7 +5743,7 @@
       <c r="M156" s="1"/>
       <c r="N156" s="1"/>
     </row>
-    <row r="157" spans="1:14" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:14" ht="174">
       <c r="A157" s="1" t="s">
         <v>14</v>
       </c>
@@ -5773,7 +5769,7 @@
       <c r="M157" s="1"/>
       <c r="N157" s="1"/>
     </row>
-    <row r="158" spans="1:14" ht="345.6" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:14" ht="405">
       <c r="A158" s="1" t="s">
         <v>14</v>
       </c>
@@ -5799,7 +5795,7 @@
       <c r="M158" s="1"/>
       <c r="N158" s="1"/>
     </row>
-    <row r="159" spans="1:14" ht="216" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:14" ht="216.75">
       <c r="A159" s="1" t="s">
         <v>14</v>
       </c>
@@ -5825,7 +5821,7 @@
       <c r="M159" s="1"/>
       <c r="N159" s="1"/>
     </row>
-    <row r="160" spans="1:14" ht="302.39999999999998" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:14" ht="332.25">
       <c r="A160" s="1" t="s">
         <v>14</v>
       </c>
@@ -5851,7 +5847,7 @@
       <c r="M160" s="1"/>
       <c r="N160" s="1"/>
     </row>
-    <row r="161" spans="1:14" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:14" ht="201.75">
       <c r="A161" s="1" t="s">
         <v>14</v>
       </c>
@@ -5877,7 +5873,7 @@
       <c r="M161" s="1"/>
       <c r="N161" s="1"/>
     </row>
-    <row r="162" spans="1:14" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:14" ht="201.75">
       <c r="A162" s="1" t="s">
         <v>14</v>
       </c>
@@ -5903,7 +5899,7 @@
       <c r="M162" s="1"/>
       <c r="N162" s="1"/>
     </row>
-    <row r="163" spans="1:14" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:14" ht="216.75">
       <c r="A163" s="1" t="s">
         <v>14</v>
       </c>
@@ -5929,7 +5925,7 @@
       <c r="M163" s="1"/>
       <c r="N163" s="1"/>
     </row>
-    <row r="164" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:14" ht="115.5">
       <c r="A164" s="1" t="s">
         <v>14</v>
       </c>
@@ -5955,7 +5951,7 @@
       <c r="M164" s="1"/>
       <c r="N164" s="1"/>
     </row>
-    <row r="165" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:14" ht="130.5">
       <c r="A165" s="1" t="s">
         <v>14</v>
       </c>
@@ -5981,7 +5977,7 @@
       <c r="M165" s="1"/>
       <c r="N165" s="1"/>
     </row>
-    <row r="166" spans="1:14" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:14" ht="188.25">
       <c r="A166" s="1" t="s">
         <v>14</v>
       </c>
@@ -6007,7 +6003,7 @@
       <c r="M166" s="1"/>
       <c r="N166" s="1"/>
     </row>
-    <row r="167" spans="1:14" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:14" ht="115.5">
       <c r="A167" s="1" t="s">
         <v>14</v>
       </c>
@@ -6033,7 +6029,7 @@
       <c r="M167" s="1"/>
       <c r="N167" s="1"/>
     </row>
-    <row r="168" spans="1:14" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:14" ht="188.25">
       <c r="A168" s="1" t="s">
         <v>14</v>
       </c>
@@ -6059,7 +6055,7 @@
       <c r="M168" s="1"/>
       <c r="N168" s="1"/>
     </row>
-    <row r="169" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:14" ht="130.5">
       <c r="A169" s="1" t="s">
         <v>14</v>
       </c>
@@ -6085,7 +6081,7 @@
       <c r="M169" s="1"/>
       <c r="N169" s="1"/>
     </row>
-    <row r="170" spans="1:14" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:14" ht="216.75">
       <c r="A170" s="1" t="s">
         <v>14</v>
       </c>
@@ -6111,7 +6107,7 @@
       <c r="M170" s="1"/>
       <c r="N170" s="1"/>
     </row>
-    <row r="171" spans="1:14" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:14" ht="260.25">
       <c r="A171" s="1" t="s">
         <v>14</v>
       </c>
@@ -6137,7 +6133,7 @@
       <c r="M171" s="1"/>
       <c r="N171" s="1"/>
     </row>
-    <row r="172" spans="1:14" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:14" ht="159">
       <c r="A172" s="1" t="s">
         <v>14</v>
       </c>
@@ -6170,14 +6166,28 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010008B6C2F7E3649F4890535B93589B6D26" ma:contentTypeVersion="4" ma:contentTypeDescription="Criar um novo documento." ma:contentTypeScope="" ma:versionID="23de76a9b7b882c75a25fec7da9a2c55">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2699dae1-7ace-4b59-8f20-7e9528f3669f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e2d70c6c1dfe9ed288ae760ac4bf1c6d" ns2:_="">
     <xsd:import namespace="2699dae1-7ace-4b59-8f20-7e9528f3669f"/>
@@ -6321,59 +6331,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58FF35FE-E478-4286-A918-088A5DD7FE3B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2699dae1-7ace-4b59-8f20-7e9528f3669f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D0DFCA6-C690-4CB2-ABF8-EAAC398B5E19}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED659437-1F5B-4C2A-96DA-B17E9F3E8592}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED659437-1F5B-4C2A-96DA-B17E9F3E8592}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D0DFCA6-C690-4CB2-ABF8-EAAC398B5E19}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="2699dae1-7ace-4b59-8f20-7e9528f3669f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58FF35FE-E478-4286-A918-088A5DD7FE3B}"/>
 </file>
</xml_diff>